<commit_message>
funcionamiento del boton busqueda de archivos
</commit_message>
<xml_diff>
--- a/out10.xlsx
+++ b/out10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,16 +467,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,21 +502,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>106</v>
+        <v>288</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/26</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,21 +537,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>108</v>
+        <v>292</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/27</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,21 +572,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>110</v>
+        <v>296</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/28</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -607,21 +607,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>112</v>
+        <v>300</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/29</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -642,21 +642,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>115</v>
+        <v>306</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -677,21 +677,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -712,21 +712,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>118</v>
+        <v>314</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -747,21 +747,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>119</v>
+        <v>318</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -782,21 +782,21 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>120</v>
+        <v>322</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -817,21 +817,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>121</v>
+        <v>326</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/35</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -852,21 +852,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>122</v>
+        <v>330</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -887,21 +887,21 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>123</v>
+        <v>334</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -922,34 +922,2099 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>124</v>
+        <v>338</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>172.30.87.56</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>xe-0/0/38</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>xe-0/0/39</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>xe-0/0/40</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>xe-0/0/41</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>xe-0/0/42</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>xe-0/0/43</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>xe-0/0/44</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>xe-0/0/45</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>xe-0/0/46</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>172.30.51.185</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>xe-0/0/48</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>xe-0/0/0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>xe-0/0/1</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>xe-0/0/10</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>xe-0/0/11</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>389</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>xe-0/0/12</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>393</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>xe-0/0/13</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>397</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>xe-0/0/14</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>xe-0/0/15</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>405</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>xe-0/0/16</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>409</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>xe-0/0/17</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>xe-0/0/18</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>417</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>xe-0/0/19</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>421</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>xe-0/0/2</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>423</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>xe-0/0/20</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>xe-0/0/21</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>431</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>xe-0/0/22</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>435</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>xe-0/0/23</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>439</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>xe-0/0/24</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>xe-0/0/25</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>xe-0/0/26</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>451</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>xe-0/0/27</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>455</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>xe-0/0/28</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>459</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>xe-0/0/29</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>460</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>xe-0/0/3</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>462</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>xe-0/0/30</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>463</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>xe-0/0/31</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>464</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>xe-0/0/32</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>465</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>xe-0/0/33</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>466</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>xe-0/0/34</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>467</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>xe-0/0/35</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>468</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>xe-0/0/36</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>xe-0/0/37</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>xe-0/0/38</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>xe-0/0/39</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>472</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>xe-0/0/4</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>474</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>xe-0/0/40</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>475</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>xe-0/0/41</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>476</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>xe-0/0/42</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>477</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>xe-0/0/43</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>478</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>xe-0/0/44</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>479</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>xe-0/0/45</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>480</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>xe-0/0/46</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>481</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>482</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>xe-0/0/48</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>484</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>xe-0/0/5</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>486</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>xe-0/0/6</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>488</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>xe-0/0/7</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>492</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>xe-0/0/8</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>496</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>xe-0/0/9</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>PUERTOLIBRE</t>
         </is>

</xml_diff>

<commit_message>
se cambia el diseño de la ventana principal
</commit_message>
<xml_diff>
--- a/out10.xlsx
+++ b/out10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,21 +467,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1233</v>
+        <v>218</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>xe-0/0/14</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,21 +502,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1234</v>
+        <v>288</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>xe-0/0/15</t>
+          <t>xe-0/0/26</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,21 +537,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1235</v>
+        <v>292</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>xe-0/0/16</t>
+          <t>xe-0/0/27</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,21 +572,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1236</v>
+        <v>296</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xe-0/0/17</t>
+          <t>xe-0/0/28</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -607,21 +607,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1237</v>
+        <v>300</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>xe-0/0/18</t>
+          <t>xe-0/0/29</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -642,21 +642,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1238</v>
+        <v>306</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>xe-0/0/19</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -677,21 +677,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1240</v>
+        <v>310</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xe-0/0/20</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -712,21 +712,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1241</v>
+        <v>314</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>xe-0/0/21</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -747,21 +747,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1242</v>
+        <v>318</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>xe-0/0/22</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -782,21 +782,21 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1243</v>
+        <v>322</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>xe-0/0/23</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -817,21 +817,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1244</v>
+        <v>326</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>xe-0/0/24</t>
+          <t>xe-0/0/35</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -852,21 +852,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1245</v>
+        <v>330</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>xe-0/0/25</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -887,21 +887,21 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1246</v>
+        <v>334</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>xe-0/0/26</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -922,21 +922,21 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1247</v>
+        <v>338</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>xe-0/0/27</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -957,21 +957,21 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1248</v>
+        <v>342</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>xe-0/0/28</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -992,21 +992,21 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1249</v>
+        <v>348</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>xe-0/0/29</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1027,21 +1027,21 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1251</v>
+        <v>352</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>xe-0/0/30</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1062,21 +1062,21 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1252</v>
+        <v>353</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>xe-0/0/31</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1097,21 +1097,21 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>1253</v>
+        <v>354</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>xe-0/0/32</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1132,21 +1132,21 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1254</v>
+        <v>355</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>xe-0/0/33</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1167,21 +1167,21 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1255</v>
+        <v>356</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>xe-0/0/34</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1202,21 +1202,21 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1257</v>
+        <v>357</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1237,21 +1237,21 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1258</v>
+        <v>358</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1272,21 +1272,21 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1259</v>
+        <v>359</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.185</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-03-DAAS</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1307,31 +1307,31 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1260</v>
+        <v>377</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>down</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>down</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1342,21 +1342,21 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1262</v>
+        <v>379</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1377,31 +1377,31 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1263</v>
+        <v>381</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/10</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>up</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>down</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1412,31 +1412,31 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1264</v>
+        <v>385</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/11</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>up</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>down</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1447,21 +1447,21 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1265</v>
+        <v>389</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1482,21 +1482,21 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1266</v>
+        <v>393</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/13</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1517,21 +1517,21 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1267</v>
+        <v>397</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1552,21 +1552,21 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1268</v>
+        <v>401</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/15</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1587,21 +1587,21 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1269</v>
+        <v>405</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/16</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1622,34 +1622,1399 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>1270</v>
+        <v>409</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.30.51.186</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>BOGO-GARCE-H-04-DAAS</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>xe-0/0/17</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>xe-0/0/18</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>417</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>xe-0/0/19</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>421</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>xe-0/0/2</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>423</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>xe-0/0/20</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>xe-0/0/21</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>431</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>xe-0/0/22</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>435</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>xe-0/0/23</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>439</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>xe-0/0/24</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>xe-0/0/25</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>xe-0/0/26</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>451</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>xe-0/0/27</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>455</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>xe-0/0/28</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>459</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>xe-0/0/29</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>460</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>xe-0/0/3</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>462</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>xe-0/0/30</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>463</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>xe-0/0/31</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>464</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>xe-0/0/32</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>465</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>xe-0/0/33</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>466</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>xe-0/0/34</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>467</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>xe-0/0/35</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>468</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>xe-0/0/36</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>xe-0/0/37</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>xe-0/0/38</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>xe-0/0/39</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>472</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>xe-0/0/4</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>474</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>xe-0/0/40</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>475</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>xe-0/0/41</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>476</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>xe-0/0/42</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>477</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>xe-0/0/43</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>478</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>xe-0/0/44</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>479</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>xe-0/0/45</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>480</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>xe-0/0/46</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>481</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>482</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
           <t>xe-0/0/48</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>484</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>xe-0/0/5</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>486</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>xe-0/0/6</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>488</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>xe-0/0/7</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>492</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>xe-0/0/8</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>496</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>172.30.51.186</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>BOGO-GARCE-H-04-DAAS</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>xe-0/0/9</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>PUERTOLIBRE</t>
         </is>

</xml_diff>

<commit_message>
Se agrego codigo del diseño de Excel
</commit_message>
<xml_diff>
--- a/out10.xlsx
+++ b/out10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,21 +467,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1233</v>
+        <v>1277</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>xe-0/0/14</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,21 +502,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1234</v>
+        <v>1321</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>xe-0/0/15</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,21 +537,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1235</v>
+        <v>1322</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>xe-0/0/16</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,21 +572,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1236</v>
+        <v>1323</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xe-0/0/17</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -607,21 +607,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1237</v>
+        <v>1324</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>xe-0/0/18</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -642,21 +642,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1238</v>
+        <v>1325</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>xe-0/0/19</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -677,21 +677,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1240</v>
+        <v>1326</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xe-0/0/20</t>
+          <t>xe-0/0/35</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -712,21 +712,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1241</v>
+        <v>1327</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>xe-0/0/21</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -747,21 +747,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1242</v>
+        <v>1328</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>xe-0/0/22</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -782,21 +782,21 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1243</v>
+        <v>1329</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>xe-0/0/23</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -817,21 +817,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1244</v>
+        <v>1330</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>xe-0/0/24</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -852,21 +852,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1245</v>
+        <v>1332</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>xe-0/0/25</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -887,21 +887,21 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1246</v>
+        <v>1333</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>xe-0/0/26</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -922,21 +922,21 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1247</v>
+        <v>1334</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>xe-0/0/27</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -957,21 +957,21 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1248</v>
+        <v>1335</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>xe-0/0/28</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -992,21 +992,21 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1249</v>
+        <v>1336</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>xe-0/0/29</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1027,21 +1027,21 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1251</v>
+        <v>1337</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>xe-0/0/30</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1062,21 +1062,21 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1252</v>
+        <v>1338</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>xe-0/0/31</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1097,21 +1097,21 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>1253</v>
+        <v>1339</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>xe-0/0/32</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1132,21 +1132,21 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1254</v>
+        <v>1340</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>xe-0/0/33</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1167,21 +1167,21 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1255</v>
+        <v>1347</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>xe-0/0/34</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1202,21 +1202,21 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1257</v>
+        <v>1399</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1237,21 +1237,21 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1258</v>
+        <v>1414</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1272,21 +1272,21 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1259</v>
+        <v>1415</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1307,21 +1307,21 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1260</v>
+        <v>1416</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1342,21 +1342,21 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1262</v>
+        <v>1417</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1377,21 +1377,21 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1263</v>
+        <v>1418</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1412,21 +1412,21 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1264</v>
+        <v>1419</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1447,21 +1447,21 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1265</v>
+        <v>1420</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1482,21 +1482,21 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1266</v>
+        <v>1421</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1517,21 +1517,21 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1267</v>
+        <v>1431</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1552,21 +1552,21 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1268</v>
+        <v>1487</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1587,21 +1587,21 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1269</v>
+        <v>1489</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1622,34 +1622,454 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>1270</v>
+        <v>1491</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>xe-0/0/38</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>1493</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>xe-0/0/39</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>1496</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>xe-0/0/40</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>1498</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>xe-0/0/41</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1499</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>xe-0/0/42</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>xe-0/0/43</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>1501</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>xe-0/0/44</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>1502</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>xe-0/0/45</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>1503</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>xe-0/0/46</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>1504</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>1505</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>xe-0/0/48</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>1507</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>xe-0/0/5</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>1509</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>xe-0/0/7</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>PUERTOLIBRE</t>
         </is>

</xml_diff>

<commit_message>
funcion simulitud de puertos
</commit_message>
<xml_diff>
--- a/out10.xlsx
+++ b/out10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,21 +467,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1233</v>
+        <v>1277</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>xe-0/0/14</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,21 +502,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1234</v>
+        <v>1321</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>xe-0/0/15</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,21 +537,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1235</v>
+        <v>1322</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>xe-0/0/16</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,21 +572,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1236</v>
+        <v>1323</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xe-0/0/17</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -607,21 +607,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1237</v>
+        <v>1324</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>xe-0/0/18</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -642,21 +642,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1238</v>
+        <v>1325</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>xe-0/0/19</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -677,21 +677,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1240</v>
+        <v>1326</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xe-0/0/20</t>
+          <t>xe-0/0/35</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -712,21 +712,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1241</v>
+        <v>1327</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>xe-0/0/21</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -747,21 +747,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1242</v>
+        <v>1328</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>xe-0/0/22</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -782,21 +782,21 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1243</v>
+        <v>1329</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>xe-0/0/23</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -817,21 +817,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1244</v>
+        <v>1330</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>xe-0/0/24</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -852,21 +852,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1245</v>
+        <v>1332</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>xe-0/0/25</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -887,21 +887,21 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1246</v>
+        <v>1333</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>xe-0/0/26</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -922,21 +922,21 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1247</v>
+        <v>1334</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>xe-0/0/27</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -957,21 +957,21 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1248</v>
+        <v>1335</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>xe-0/0/28</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -992,21 +992,21 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1249</v>
+        <v>1336</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>xe-0/0/29</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1027,21 +1027,21 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1251</v>
+        <v>1337</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>xe-0/0/30</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1062,21 +1062,21 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1252</v>
+        <v>1338</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>xe-0/0/31</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1097,21 +1097,21 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>1253</v>
+        <v>1339</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>xe-0/0/32</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1132,21 +1132,21 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1254</v>
+        <v>1340</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-01-DAAS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>xe-0/0/33</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1167,21 +1167,21 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1255</v>
+        <v>1347</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>xe-0/0/34</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1202,21 +1202,21 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1257</v>
+        <v>1399</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1237,21 +1237,21 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1258</v>
+        <v>1414</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1272,21 +1272,21 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1259</v>
+        <v>1415</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1307,21 +1307,21 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1260</v>
+        <v>1416</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1342,21 +1342,21 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1262</v>
+        <v>1417</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1377,21 +1377,21 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1263</v>
+        <v>1418</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1412,21 +1412,21 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1264</v>
+        <v>1419</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1447,21 +1447,21 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1265</v>
+        <v>1420</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1482,21 +1482,21 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1266</v>
+        <v>1421</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.24</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-02-DAAS</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1517,21 +1517,21 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1267</v>
+        <v>1431</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1552,21 +1552,21 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1268</v>
+        <v>1487</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1587,21 +1587,21 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1269</v>
+        <v>1489</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1622,34 +1622,454 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>1270</v>
+        <v>1491</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>172.28.255.41</t>
+          <t>172.24.254.25</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
+          <t>MEDE-CABA-H-03-DAAS</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>xe-0/0/38</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>1493</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>xe-0/0/39</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>1496</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>xe-0/0/40</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>1498</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>xe-0/0/41</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1499</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>xe-0/0/42</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>xe-0/0/43</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>1501</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>xe-0/0/44</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>1502</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>xe-0/0/45</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>1503</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>xe-0/0/46</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>1504</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>1505</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>xe-0/0/48</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>1507</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>xe-0/0/5</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>1509</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>172.24.254.25</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-03-DAAS</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>xe-0/0/7</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>PUERTOLIBRE</t>
         </is>

</xml_diff>